<commit_message>
arreglado opcion de cargar datos en caso de error
</commit_message>
<xml_diff>
--- a/resultados/resultado_prueba.xlsx
+++ b/resultados/resultado_prueba.xlsx
@@ -537,21 +537,21 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>30U1YOGZGAW71ZX6E9LWKLA5JD8SDZ</t>
+          <t>301KG0KX9CLV8GLA6QPGKOCZD972HG</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>having a great and high wall; having twelve gates, and at the gates twelve angels; and names written on them, which are the names of the twelve tribes of the children of Israel.</t>
+          <t>At the evening offering I arose up from my humiliation, even with my garment and my robe torn; and I fell on my knees, and spread out my hands to Yahweh my God;</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>tribes</t>
+          <t>garment</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -565,10 +565,10 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.03518308700730965</v>
+        <v>0.2499896965645608</v>
       </c>
       <c r="H2" t="n">
-        <v>0.175</v>
+        <v>0.21875</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -581,41 +581,41 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N2" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O2" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P2" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>easy:85.93%</t>
+          <t>neutral:0.74%</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>neutral:9.47%</t>
+          <t>Easy:0.01%</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>difficult:3.2%</t>
+          <t>easy:0.0%</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>very:0.9%</t>
+          <t>:0.0%</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -626,42 +626,42 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>30UZJB2POHC8D5XY9O2CE1E1EE6533</t>
+          <t>301KG0KX9CLV8GLA6QPGKOCZD9X2H6</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>so that the multitude wondered when they saw the mute speaking, injured whole, lame walking, and blind seeing--and they glorified the God of Israel.</t>
+          <t>It shall be to them as a false divination in their sight, who have sworn oaths to them; but he brings iniquity to memory, that they may be taken.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>whole</t>
+          <t>divination</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>easy</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.01 - 0.25</t>
+          <t>0.26 - 0.5</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.2497868900824576</v>
+        <v>0.375</v>
       </c>
       <c r="H3" t="n">
-        <v>0.359375</v>
+        <v>0.638888918</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>difficult</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -670,41 +670,41 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N3" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>very:5.83%</t>
+          <t>neutral:84.37%</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>neutral:2.29%</t>
+          <t>difficult:10.64%</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Easy:0.11%</t>
+          <t>easy:4.89%</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>easy:0.09%</t>
+          <t>Neutral:0.07%</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -715,38 +715,38 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>30UZJB2POHC8D5XY9O2CE1E1EEG35B</t>
+          <t>301KG0KX9CLV8GLA6QPGKOCZDB2H2U</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>In that day, Yahweh with his hard and great and strong sword will punish leviathan, the fleeing serpent, and leviathan the twisted serpent; and he will kill the dragon that is in the sea.</t>
+          <t>You have received gifts among men, yes, among the rebellious also, that Yah God might dwell there.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>dragon</t>
+          <t>gifts</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>difficult</t>
+          <t>easy</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.51 - 0.75</t>
+          <t>0.01 - 0.25</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.6828580984705551</v>
+        <v>0.2499889281109571</v>
       </c>
       <c r="H4" t="n">
-        <v>0.25</v>
+        <v>0.08928568200000001</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -755,45 +755,45 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N4" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O4" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P4" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>difficult:69.14%</t>
+          <t>neutral:0.93%</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>easy:15.66%</t>
+          <t>Easy:0.01%</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>neutral:11.48%</t>
+          <t>very:0.01%</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>very:3.34%</t>
+          <t>easy:0.0%</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -804,21 +804,21 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>30UZJB2POHC8D5XY9O2CE1E1EEG53D</t>
+          <t>301KG0KX9CLV8GLA6QPGKOCZDBWH2O</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Then arose Ishmael the son of Nethaniah, and the ten men who were with him, and struck Gedaliah the son of Ahikam the son of Shaphan with the sword, and killed him, whom the king of Babylon had made governor over the land.</t>
+          <t>Therefore he poured the fierceness of his anger on him, and the strength of battle; and it set him on fire all around, but he didn't know; and it burned him, but he didn't take it to heart."</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>king</t>
+          <t>strength</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -832,10 +832,10 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0.0621026209156138</v>
+        <v>0.2499878463276225</v>
       </c>
       <c r="H5" t="n">
-        <v>0.107142816</v>
+        <v>0.166666648</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -848,66 +848,66 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N5" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O5" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P5" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>easy:75.16%</t>
+          <t>neutral:14.04%</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>very:22.75%</t>
+          <t>Easy:0.02%</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>neutral:1.67%</t>
+          <t>Neutral:0.01%</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Easy:0.11%</t>
+          <t>easy:0.0%</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>difficult:0.06%</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>30UZJB2POHC8D5XY9O2CE1E1EEU53R</t>
+          <t>301KG0KX9CLV8GLA6QPGKOCZDBX2HA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Yahweh will bring you, and your king whom you shall set over you, to a nation that you have not known, you nor your fathers; and there you shall serve other gods, wood and stone.</t>
+          <t>The seventh angel sounded, and great voices in heaven followed, saying, "The kingdom of the world has become the Kingdom of our Lord, and of his Christ.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>wood</t>
+          <t>voices</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -921,10 +921,10 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.06306167532861912</v>
+        <v>0.2499884037545524</v>
       </c>
       <c r="H6" t="n">
-        <v>0.117647062</v>
+        <v>0.18421044</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -937,41 +937,41 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N6" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O6" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P6" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>easy:74.78%</t>
+          <t>neutral:1.48%</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>neutral:14.52%</t>
+          <t>Easy:0.02%</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>very:9.37%</t>
+          <t>easy:0.0%</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>difficult:0.91%</t>
+          <t>Neutral:0.0%</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -982,21 +982,21 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>30UZJB2POHC8D5XY9O2CE1E1EG6355</t>
+          <t>302OLP89DZ7TWB5YXD4UFFYHC58AC0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>They couldn't find what they might do, for all the people hung on to every word that he said.</t>
+          <t>who by the mouth of your servant, David, said, 'Why do the nations rage, and the peoples plot a vain thing?</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>rage</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1010,10 +1010,10 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0.05422733808276603</v>
+        <v>0.2499853649494029</v>
       </c>
       <c r="H7" t="n">
-        <v>0.161764642</v>
+        <v>0.214285633</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -1026,41 +1026,41 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N7" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O7" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P7" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>easy:78.31%</t>
+          <t>neutral:2.84%</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>very:13.4%</t>
+          <t>Easy:0.02%</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>neutral:7.98%</t>
+          <t>Neutral:0.01%</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>Easy:0.14%</t>
+          <t>easy:0.01%</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -1071,38 +1071,38 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>30UZJB2POHC8D5XY9O2CE1E1EG6537</t>
+          <t>302OLP89DZ7TWB5YXD4UFFYHC5KCAE</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>God said, "Let there be an expanse in the middle of the waters, and let it divide the waters from the waters."</t>
+          <t>'You shall keep my Sabbaths, and reverence my sanctuary; I am Yahweh.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>expanse</t>
+          <t>Sabbaths</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>difficult</t>
+          <t>easy</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.51 - 0.75</t>
+          <t>0.01 - 0.25</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0.6152658250323791</v>
+        <v>0.2499822299869348</v>
       </c>
       <c r="H8" t="n">
-        <v>0.274999898</v>
+        <v>0.34375</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -1115,41 +1115,41 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M8" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N8" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O8" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P8" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>difficult:42.11%</t>
+          <t>neutral:1.09%</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>neutral:34.15%</t>
+          <t>Easy:0.03%</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>easy:20.75%</t>
+          <t>easy:0.01%</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>very:2.25%</t>
+          <t>Neutral:0.01%</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1160,21 +1160,21 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>30Y6N4AHYPWV0KXTZKLRUB59X9CRDT</t>
+          <t>302OLP89DZ7TWB5YXD4UFFYHC7KACG</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>and all the storage cities that Solomon had, and the cities for his chariots, and the cities for his horsemen, and that which Solomon desired to build for his pleasure in Jerusalem, and in Lebanon, and in all the land of his dominion.</t>
+          <t>Neither have we inheritance in the son of Jesse!</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>Jesse</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1188,10 +1188,10 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>0.06224280955963402</v>
+        <v>0.009698101353405764</v>
       </c>
       <c r="H9" t="n">
-        <v>0.3</v>
+        <v>0.323529285</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -1204,66 +1204,66 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M9" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N9" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O9" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P9" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>easy:75.1%</t>
+          <t>easy:96.12%</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>neutral:16.99%</t>
+          <t>neutral:3.76%</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>very:4.21%</t>
+          <t>very:0.08%</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>difficult:3.09%</t>
+          <t>Easy:0.02%</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Neutral:0.01%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>30Y6N4AHYPWV0KXTZKLRUB59XBJRD4</t>
+          <t>302OLP89DZ7TWB5YXD4UFFYHC7PCAN</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>on the south; all the land of the Canaanites, and Mearah that belongs to the Sidonians, to Aphek, to the border of the Amorites;</t>
+          <t>Only the firstborn among animals, which is made a firstborn to Yahweh, no man may dedicate it; whether an ox or sheep, it is Yahweh's.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Canaanites</t>
+          <t>animals</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1277,57 +1277,57 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0.1241874931479697</v>
+        <v>0.2499928275566013</v>
       </c>
       <c r="H10" t="n">
-        <v>0.410714191</v>
+        <v>0.222222222</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>easy</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M10" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N10" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O10" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P10" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>easy:50.33%</t>
+          <t>neutral:0.49%</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>difficult:31.31%</t>
+          <t>very:0.03%</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>neutral:9.43%</t>
+          <t>Easy:0.01%</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>very:8.25%</t>
+          <t>easy:0.0%</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -1338,85 +1338,85 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>30Y6N4AHYPWV0KXTZKLRUB59XBKDRR</t>
+          <t>302U8RURJZ1WF35NXY44RD66WJ8NVH</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>But beware of men: for they will deliver you up to councils, and in their synagogues they will scourge you.</t>
+          <t>Don't be desirous of his dainties, since they are deceitful food.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>synagogues</t>
+          <t>dainties</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.26 - 0.5</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.638888918</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
           <t>difficult</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0.51 - 0.75</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>0.671888443533696</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.51470574</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>difficult</t>
-        </is>
-      </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M11" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N11" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O11" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P11" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>difficult:64.76%</t>
+          <t>neutral:81.26%</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>neutral:19.02%</t>
+          <t>easy:17.86%</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>easy:14.12%</t>
+          <t>difficult:0.81%</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>very:1.39%</t>
+          <t>Neutral:0.06%</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -1427,85 +1427,85 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>30Z7M1Q8UYKRK8FLG1OPDT2YMENA8U</t>
+          <t>302U8RURJZ1WF35NXY44RD66WJ8VNP</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Now accept one who is weak in faith, but not for disputes over opinions.</t>
+          <t>The floods have lifted up, Yahweh, the floods have lifted up their voice.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>disputes</t>
+          <t>voice</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>easy</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0.01 - 0.25</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0.249989758317862</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.266666692</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
           <t>neutral</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>0.26 - 0.5</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.283333343</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>0.1825</v>
+        <v>0.1233</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0476</v>
+        <v>0.0261</v>
       </c>
       <c r="M12" t="n">
-        <v>0.2182</v>
+        <v>0.1615</v>
       </c>
       <c r="N12" t="n">
-        <v>-2.2824</v>
+        <v>0.1274</v>
       </c>
       <c r="O12" t="n">
-        <v>0.5201</v>
+        <v>0.4622</v>
       </c>
       <c r="P12" t="n">
-        <v>0.5182</v>
+        <v>0.3333</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>neutral:34.45%</t>
+          <t>neutral:0.75%</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>easy:33.14%</t>
+          <t>very:0.22%</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>difficult:31.34%</t>
+          <t>Easy:0.02%</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>very:0.45%</t>
+          <t>easy:0.0%</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">

</xml_diff>